<commit_message>
need to be clean up
</commit_message>
<xml_diff>
--- a/data-portal-list.xlsx
+++ b/data-portal-list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1152" windowWidth="30720" windowHeight="13524" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="1728" windowWidth="30720" windowHeight="13524" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="中央" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="952">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="972">
   <si>
     <t>OID</t>
   </si>
@@ -2882,6 +2882,66 @@
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>https://data.moi.gov.tw/</t>
+  </si>
+  <si>
+    <t>https://www.boca.gov.tw/lp-opendata-All-1.html</t>
+  </si>
+  <si>
+    <t>外交部_領事事務局</t>
+  </si>
+  <si>
+    <t>https://ahonline.drnh.gov.tw/index.php?act=Archive</t>
+  </si>
+  <si>
+    <t>國史館_台灣文獻館</t>
+  </si>
+  <si>
+    <t>http://ds3.th.gov.tw/ds3</t>
+  </si>
+  <si>
+    <t>https://www.th.gov.tw/</t>
+  </si>
+  <si>
+    <t>https://data.coa.gov.tw/</t>
+  </si>
+  <si>
+    <t>https://opendata.epa.gov.tw/</t>
+  </si>
+  <si>
+    <t>https://opendata.culture.tw/</t>
+  </si>
+  <si>
+    <t>http://theme.npm.edu.tw/opendata/</t>
+  </si>
+  <si>
+    <t>https://data.gov.tw/</t>
+  </si>
+  <si>
+    <t>http://data.hakka.gov.tw/</t>
+  </si>
+  <si>
+    <t>https://www.vac.gov.tw/lp-opendata-All-1-1-40.html</t>
+  </si>
+  <si>
+    <t>https://www.ocac.gov.tw/OCAC/Pages/List.aspx?nodeid=353</t>
+  </si>
+  <si>
+    <t>https://www.cga.gov.tw/GipOpen/wSite/lp?ctNode=8871&amp;mp=9996</t>
+  </si>
+  <si>
+    <t>https://web3.dgpa.gov.tw/WANT03FRONT/AP/WANTF00003.aspx</t>
+  </si>
+  <si>
+    <t>https://www.aec.gov.tw/%E8%B3%87%E8%A8%8A%E5%85%AC%E9%96%8B/%E9%96%8B%E6%94%BE%E8%B3%87%E6%96%99-Open-Data--219_2015.html</t>
+  </si>
+  <si>
+    <t>http://db.cec.gov.tw/</t>
+  </si>
+  <si>
+    <t>https://www.ncc.gov.tw/chinese/opendata.aspx</t>
   </si>
 </sst>
 </file>
@@ -2951,7 +3011,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2992,6 +3052,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3273,23 +3334,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I65"/>
+  <dimension ref="A1:I67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K44" sqref="K44"/>
+      <selection pane="bottomRight" activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.77734375" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="9.21875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="23.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="27.77734375" style="3" customWidth="1"/>
     <col min="4" max="4" width="50.21875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="31.21875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="46.33203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="7.88671875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="56" style="3" customWidth="1"/>
     <col min="7" max="7" width="56.5546875" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.6640625" style="8" customWidth="1"/>
     <col min="9" max="9" width="10.88671875" style="8" customWidth="1"/>
@@ -3368,6 +3429,9 @@
       <c r="D4" s="5" t="s">
         <v>76</v>
       </c>
+      <c r="F4" s="3" t="s">
+        <v>955</v>
+      </c>
       <c r="G4" s="6" t="s">
         <v>185</v>
       </c>
@@ -3380,805 +3444,841 @@
     </row>
     <row r="5" spans="1:9">
       <c r="C5" s="4" t="s">
+        <v>956</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>958</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>957</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="12"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D6" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H6" s="12" t="s">
         <v>274</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I6" s="8">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
-      <c r="B6" s="4" t="s">
+    <row r="7" spans="1:9">
+      <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5" t="s">
+      <c r="C7" s="4"/>
+      <c r="D7" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G7" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H7" s="12" t="s">
         <v>275</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I7" s="8">
         <v>21018</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="C7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>276</v>
-      </c>
-      <c r="I7" s="8">
-        <v>972</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="C8" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>952</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I8" s="8">
-        <v>141</v>
+        <v>972</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="C9" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I9" s="8">
-        <v>363</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="C10" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>279</v>
-      </c>
-      <c r="I10" s="8">
-        <v>2156</v>
-      </c>
+        <v>954</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="F10" s="3" t="s">
+        <v>953</v>
+      </c>
+      <c r="G10" s="6"/>
+      <c r="H10" s="12"/>
     </row>
     <row r="11" spans="1:9">
       <c r="C11" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="I11" s="8">
-        <v>961</v>
+        <v>363</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="C12" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>243</v>
+        <v>261</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="I12" s="8">
-        <v>2040</v>
+        <v>2156</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="C13" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="I13" s="8">
-        <v>2447</v>
+        <v>961</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="C14" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="I14" s="8">
-        <v>1379</v>
+        <v>2040</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="C15" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>232</v>
+        <v>247</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="I15" s="8">
-        <v>567</v>
+        <v>2447</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="C16" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>259</v>
+        <v>230</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="I16" s="8">
-        <v>1159</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="17" spans="3:9">
       <c r="C17" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>260</v>
+        <v>232</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="I17" s="8">
-        <v>1318</v>
+        <v>567</v>
       </c>
     </row>
     <row r="18" spans="3:9">
       <c r="C18" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>959</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="I18" s="8">
-        <v>1149</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="19" spans="3:9">
       <c r="C19" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>242</v>
+        <v>260</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="I19" s="8">
-        <v>360</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="20" spans="3:9">
       <c r="C20" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>960</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>246</v>
+        <v>258</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="I20" s="8">
-        <v>365</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="21" spans="3:9">
       <c r="C21" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>961</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>227</v>
+        <v>242</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="I21" s="8">
-        <v>512</v>
+        <v>360</v>
       </c>
     </row>
     <row r="22" spans="3:9">
       <c r="C22" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="I22" s="8">
-        <v>216</v>
+        <v>365</v>
       </c>
     </row>
     <row r="23" spans="3:9">
       <c r="C23" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>963</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>262</v>
+        <v>227</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="I23" s="8">
-        <v>1410</v>
+        <v>512</v>
       </c>
     </row>
     <row r="24" spans="3:9">
       <c r="C24" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H24" s="12" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="I24" s="8">
-        <v>115</v>
+        <v>216</v>
       </c>
     </row>
     <row r="25" spans="3:9">
       <c r="C25" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>235</v>
+        <v>262</v>
       </c>
       <c r="H25" s="12" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="I25" s="8">
-        <v>131</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="26" spans="3:9">
       <c r="C26" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>967</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>237</v>
+        <v>257</v>
       </c>
       <c r="H26" s="12" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="I26" s="8">
-        <v>170</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="3:9">
       <c r="C27" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>966</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="H27" s="12" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="I27" s="8">
-        <v>213</v>
+        <v>131</v>
       </c>
     </row>
     <row r="28" spans="3:9">
       <c r="C28" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>965</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="H28" s="12" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="I28" s="8">
-        <v>150</v>
+        <v>170</v>
       </c>
     </row>
     <row r="29" spans="3:9">
       <c r="C29" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>254</v>
+        <v>234</v>
       </c>
       <c r="H29" s="12" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="I29" s="8">
-        <v>157</v>
+        <v>213</v>
       </c>
     </row>
     <row r="30" spans="3:9">
       <c r="C30" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>964</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="H30" s="12" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="I30" s="8">
-        <v>1245</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" spans="3:9">
       <c r="C31" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="I31" s="8">
-        <v>150</v>
+        <v>157</v>
       </c>
     </row>
     <row r="32" spans="3:9">
       <c r="C32" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>231</v>
+        <v>252</v>
       </c>
       <c r="H32" s="12" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="I32" s="8">
-        <v>261</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="33" spans="2:9">
       <c r="C33" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>968</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>228</v>
+        <v>253</v>
       </c>
       <c r="H33" s="12" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="I33" s="8">
-        <v>107</v>
+        <v>150</v>
       </c>
     </row>
     <row r="34" spans="2:9">
       <c r="C34" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>255</v>
+        <v>231</v>
       </c>
       <c r="H34" s="12" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="I34" s="8">
-        <v>121</v>
+        <v>261</v>
       </c>
     </row>
     <row r="35" spans="2:9">
       <c r="C35" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D35" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>962</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="H35" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="I35" s="8">
         <v>107</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="H35" s="12" t="s">
-        <v>304</v>
-      </c>
-      <c r="I35" s="8">
-        <v>38</v>
       </c>
     </row>
     <row r="36" spans="2:9">
       <c r="C36" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>969</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>233</v>
+        <v>255</v>
       </c>
       <c r="H36" s="12" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="I36" s="8">
-        <v>155</v>
+        <v>121</v>
       </c>
     </row>
     <row r="37" spans="2:9">
       <c r="C37" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>970</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="H37" s="12" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="I37" s="8">
-        <v>212</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="2:9">
       <c r="C38" s="4" t="s">
-        <v>263</v>
+        <v>38</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>265</v>
+        <v>108</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>264</v>
+        <v>233</v>
       </c>
       <c r="H38" s="12" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="I38" s="8">
-        <v>5</v>
+        <v>155</v>
       </c>
     </row>
     <row r="39" spans="2:9">
       <c r="C39" s="4" t="s">
-        <v>224</v>
+        <v>39</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>266</v>
+        <v>109</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>971</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H39" s="12" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="I39" s="8">
-        <v>3</v>
+        <v>212</v>
       </c>
     </row>
     <row r="40" spans="2:9">
       <c r="C40" s="4" t="s">
-        <v>245</v>
+        <v>263</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>244</v>
+        <v>264</v>
       </c>
       <c r="H40" s="12" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="I40" s="8">
-        <v>60</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="2:9">
       <c r="C41" s="4" t="s">
-        <v>248</v>
+        <v>224</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>249</v>
+        <v>225</v>
       </c>
       <c r="H41" s="12" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="I41" s="8">
-        <v>43</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="2:9">
       <c r="C42" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="H42" s="12" t="s">
+        <v>309</v>
+      </c>
+      <c r="I42" s="8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9">
+      <c r="C43" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="H43" s="12" t="s">
+        <v>310</v>
+      </c>
+      <c r="I43" s="8">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9">
+      <c r="C44" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D44" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="G42" s="6" t="s">
+      <c r="G44" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="H42" s="12" t="s">
+      <c r="H44" s="12" t="s">
         <v>311</v>
       </c>
-      <c r="I42" s="8">
+      <c r="I44" s="8">
         <v>59</v>
       </c>
     </row>
-    <row r="43" spans="2:9">
-      <c r="B43" s="4" t="s">
+    <row r="45" spans="2:9">
+      <c r="B45" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C43" s="4"/>
-      <c r="D43" s="5" t="s">
+      <c r="C45" s="4"/>
+      <c r="D45" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="F43" s="6" t="s">
+      <c r="F45" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="G43" s="6" t="s">
+      <c r="G45" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="H43" s="12" t="s">
+      <c r="H45" s="12" t="s">
         <v>312</v>
       </c>
-      <c r="I43" s="8">
+      <c r="I45" s="8">
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="2:9">
-      <c r="B44" s="4" t="s">
+    <row r="46" spans="2:9">
+      <c r="B46" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C44" s="4"/>
-      <c r="D44" s="5" t="s">
+      <c r="C46" s="4"/>
+      <c r="D46" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="G44" s="6" t="s">
+      <c r="G46" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="H44" s="12" t="s">
+      <c r="H46" s="12" t="s">
         <v>313</v>
       </c>
-      <c r="I44" s="8">
+      <c r="I46" s="8">
         <v>1821</v>
-      </c>
-    </row>
-    <row r="45" spans="2:9">
-      <c r="B45" s="4"/>
-      <c r="C45" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="G45" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="H45" s="12" t="s">
-        <v>314</v>
-      </c>
-      <c r="I45" s="11">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="46" spans="2:9">
-      <c r="B46" s="4"/>
-      <c r="C46" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="G46" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="H46" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="I46" s="11">
-        <v>11</v>
       </c>
     </row>
     <row r="47" spans="2:9">
       <c r="B47" s="4"/>
       <c r="C47" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H47" s="12" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="I47" s="11">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="48" spans="2:9">
       <c r="B48" s="4"/>
       <c r="C48" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H48" s="12" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="I48" s="11">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="49" spans="2:9">
       <c r="B49" s="4"/>
       <c r="C49" s="4" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H49" s="12" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="I49" s="11">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="50" spans="2:9">
       <c r="B50" s="4"/>
       <c r="C50" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H50" s="12" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="I50" s="11">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="51" spans="2:9">
       <c r="B51" s="4"/>
       <c r="C51" s="4" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H51" s="12" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="I51" s="11">
-        <v>37</v>
+        <v>12</v>
       </c>
     </row>
     <row r="52" spans="2:9">
       <c r="B52" s="4"/>
       <c r="C52" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H52" s="12" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="I52" s="11">
         <v>16</v>
@@ -4187,203 +4287,233 @@
     <row r="53" spans="2:9">
       <c r="B53" s="4"/>
       <c r="C53" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H53" s="12" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="I53" s="11">
-        <v>14</v>
+        <v>37</v>
       </c>
     </row>
     <row r="54" spans="2:9">
       <c r="B54" s="4"/>
       <c r="C54" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H54" s="12" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="I54" s="11">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="55" spans="2:9">
       <c r="B55" s="4"/>
       <c r="C55" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H55" s="12" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="I55" s="11">
-        <v>741</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56" spans="2:9">
       <c r="B56" s="4"/>
       <c r="C56" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="H56" s="12" t="s">
+        <v>323</v>
+      </c>
+      <c r="I56" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9">
+      <c r="B57" s="4"/>
+      <c r="C57" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="H57" s="12" t="s">
+        <v>324</v>
+      </c>
+      <c r="I57" s="11">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="58" spans="2:9">
+      <c r="B58" s="4"/>
+      <c r="C58" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="G56" s="6" t="s">
+      <c r="G58" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="H56" s="12" t="s">
+      <c r="H58" s="12" t="s">
         <v>325</v>
       </c>
-      <c r="I56" s="11">
+      <c r="I58" s="11">
         <v>27</v>
-      </c>
-    </row>
-    <row r="57" spans="2:9">
-      <c r="B57" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C57" s="4"/>
-      <c r="D57" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="G57" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="H57" s="12" t="s">
-        <v>326</v>
-      </c>
-      <c r="I57" s="8">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="58" spans="2:9">
-      <c r="C58" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="G58" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="H58" s="12" t="s">
-        <v>327</v>
-      </c>
-      <c r="I58" s="8">
-        <v>57</v>
       </c>
     </row>
     <row r="59" spans="2:9">
       <c r="B59" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C59" s="4"/>
       <c r="D59" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="H59" s="12" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="I59" s="8">
-        <v>207</v>
+        <v>96</v>
       </c>
     </row>
     <row r="60" spans="2:9">
       <c r="C60" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D60" s="4" t="s">
-        <v>115</v>
+        <v>43</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>113</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="H60" s="12" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="I60" s="8">
-        <v>118</v>
+        <v>57</v>
       </c>
     </row>
     <row r="61" spans="2:9">
-      <c r="C61" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D61" s="4" t="s">
-        <v>115</v>
+      <c r="B61" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C61" s="4"/>
+      <c r="D61" s="5" t="s">
+        <v>114</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="H61" s="12" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="I61" s="8">
-        <v>32</v>
+        <v>207</v>
       </c>
     </row>
     <row r="62" spans="2:9">
       <c r="C62" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>115</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H62" s="12" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="I62" s="8">
-        <v>25</v>
+        <v>118</v>
       </c>
     </row>
     <row r="63" spans="2:9">
       <c r="C63" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>115</v>
       </c>
       <c r="G63" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="H63" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="I63" s="8">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9">
+      <c r="C64" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G64" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="H64" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="I64" s="8">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="65" spans="2:9">
+      <c r="C65" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G65" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="H63" s="12" t="s">
+      <c r="H65" s="12" t="s">
         <v>332</v>
       </c>
-      <c r="I63" s="8">
+      <c r="I65" s="8">
         <v>18</v>
       </c>
     </row>
-    <row r="64" spans="2:9">
-      <c r="B64" s="3" t="s">
+    <row r="66" spans="2:9">
+      <c r="B66" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="D64" s="6" t="s">
+      <c r="D66" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="G64" s="6" t="s">
+      <c r="G66" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="H64" s="12" t="s">
+      <c r="H66" s="12" t="s">
         <v>333</v>
       </c>
-      <c r="I64" s="8">
+      <c r="I66" s="8">
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="7:7">
-      <c r="G65" s="3" t="s">
+    <row r="67" spans="2:9">
+      <c r="G67" s="3" t="s">
         <v>270</v>
       </c>
     </row>
@@ -4392,116 +4522,117 @@
     <hyperlink ref="D2" r:id="rId1"/>
     <hyperlink ref="D3" r:id="rId2"/>
     <hyperlink ref="D4" r:id="rId3"/>
-    <hyperlink ref="D5" r:id="rId4"/>
-    <hyperlink ref="D6" r:id="rId5"/>
-    <hyperlink ref="D7" r:id="rId6"/>
-    <hyperlink ref="D8" r:id="rId7"/>
-    <hyperlink ref="D9" r:id="rId8"/>
-    <hyperlink ref="D10" r:id="rId9"/>
-    <hyperlink ref="D11" r:id="rId10"/>
-    <hyperlink ref="D12" r:id="rId11"/>
-    <hyperlink ref="D13" r:id="rId12"/>
-    <hyperlink ref="D14" r:id="rId13"/>
-    <hyperlink ref="D15" r:id="rId14"/>
-    <hyperlink ref="D16" r:id="rId15"/>
-    <hyperlink ref="D17" r:id="rId16"/>
-    <hyperlink ref="D18" r:id="rId17"/>
-    <hyperlink ref="D19" r:id="rId18"/>
-    <hyperlink ref="D58" r:id="rId19"/>
-    <hyperlink ref="D59" r:id="rId20"/>
-    <hyperlink ref="D57" r:id="rId21"/>
-    <hyperlink ref="D44" r:id="rId22"/>
-    <hyperlink ref="D43" r:id="rId23"/>
-    <hyperlink ref="D37" r:id="rId24"/>
-    <hyperlink ref="D36" r:id="rId25"/>
-    <hyperlink ref="D35" r:id="rId26"/>
-    <hyperlink ref="D34" r:id="rId27"/>
-    <hyperlink ref="D33" r:id="rId28"/>
-    <hyperlink ref="D32" r:id="rId29"/>
-    <hyperlink ref="D31" r:id="rId30"/>
-    <hyperlink ref="D30" r:id="rId31"/>
-    <hyperlink ref="D29" r:id="rId32"/>
-    <hyperlink ref="D28" r:id="rId33"/>
-    <hyperlink ref="D27" r:id="rId34"/>
-    <hyperlink ref="D26" r:id="rId35"/>
-    <hyperlink ref="D25" r:id="rId36"/>
-    <hyperlink ref="D24" r:id="rId37"/>
-    <hyperlink ref="D23" r:id="rId38"/>
-    <hyperlink ref="D22" r:id="rId39"/>
-    <hyperlink ref="D21" r:id="rId40"/>
-    <hyperlink ref="D20" r:id="rId41"/>
-    <hyperlink ref="F43" r:id="rId42"/>
-    <hyperlink ref="D40" r:id="rId43"/>
-    <hyperlink ref="D42" r:id="rId44"/>
+    <hyperlink ref="D6" r:id="rId4"/>
+    <hyperlink ref="D7" r:id="rId5"/>
+    <hyperlink ref="D8" r:id="rId6"/>
+    <hyperlink ref="D9" r:id="rId7"/>
+    <hyperlink ref="D11" r:id="rId8"/>
+    <hyperlink ref="D12" r:id="rId9"/>
+    <hyperlink ref="D13" r:id="rId10"/>
+    <hyperlink ref="D14" r:id="rId11"/>
+    <hyperlink ref="D15" r:id="rId12"/>
+    <hyperlink ref="D16" r:id="rId13"/>
+    <hyperlink ref="D17" r:id="rId14"/>
+    <hyperlink ref="D18" r:id="rId15"/>
+    <hyperlink ref="D19" r:id="rId16"/>
+    <hyperlink ref="D20" r:id="rId17"/>
+    <hyperlink ref="D21" r:id="rId18"/>
+    <hyperlink ref="D60" r:id="rId19"/>
+    <hyperlink ref="D61" r:id="rId20"/>
+    <hyperlink ref="D59" r:id="rId21"/>
+    <hyperlink ref="D46" r:id="rId22"/>
+    <hyperlink ref="D45" r:id="rId23"/>
+    <hyperlink ref="D39" r:id="rId24"/>
+    <hyperlink ref="D38" r:id="rId25"/>
+    <hyperlink ref="D37" r:id="rId26"/>
+    <hyperlink ref="D36" r:id="rId27"/>
+    <hyperlink ref="D35" r:id="rId28"/>
+    <hyperlink ref="D34" r:id="rId29"/>
+    <hyperlink ref="D33" r:id="rId30"/>
+    <hyperlink ref="D32" r:id="rId31"/>
+    <hyperlink ref="D31" r:id="rId32"/>
+    <hyperlink ref="D30" r:id="rId33"/>
+    <hyperlink ref="D29" r:id="rId34"/>
+    <hyperlink ref="D28" r:id="rId35"/>
+    <hyperlink ref="D27" r:id="rId36"/>
+    <hyperlink ref="D26" r:id="rId37"/>
+    <hyperlink ref="D25" r:id="rId38"/>
+    <hyperlink ref="D24" r:id="rId39"/>
+    <hyperlink ref="D23" r:id="rId40"/>
+    <hyperlink ref="D22" r:id="rId41"/>
+    <hyperlink ref="F45" r:id="rId42"/>
+    <hyperlink ref="D42" r:id="rId43"/>
+    <hyperlink ref="D44" r:id="rId44"/>
     <hyperlink ref="G2" r:id="rId45"/>
     <hyperlink ref="G3" r:id="rId46" display="https://data.gov.tw/datasets/search?qs=dtid:800 "/>
     <hyperlink ref="G4" r:id="rId47" display="https://data.gov.tw/datasets/search?qs=dtid:723 "/>
-    <hyperlink ref="G5" r:id="rId48" display="https://data.gov.tw/datasets/search?qs=dtid:739 "/>
-    <hyperlink ref="G6" r:id="rId49" display="https://data.gov.tw/datasets/search?qs=dtid:428 "/>
-    <hyperlink ref="G7" r:id="rId50" display="https://data.gov.tw/datasets/search?qs=dtid:429 "/>
-    <hyperlink ref="G8" r:id="rId51" display="https://data.gov.tw/datasets/search?qs=dtid:430 "/>
-    <hyperlink ref="G9" r:id="rId52" display="https://data.gov.tw/datasets/search?qs=dtid:431 "/>
-    <hyperlink ref="G10" r:id="rId53" display="https://data.gov.tw/datasets/search?qs=dtid:432 "/>
-    <hyperlink ref="G11" r:id="rId54" display="https://data.gov.tw/datasets/search?qs=dtid:440 "/>
-    <hyperlink ref="G12" r:id="rId55" display="https://data.gov.tw/datasets/search?qs=dtid:442 "/>
-    <hyperlink ref="G13" r:id="rId56" display="https://data.gov.tw/datasets/search?qs=dtid:443 "/>
-    <hyperlink ref="G14" r:id="rId57" display="https://data.gov.tw/datasets/search?qs=dtid:466 "/>
-    <hyperlink ref="G15" r:id="rId58" display="https://data.gov.tw/datasets/search?qs=dtid:497 "/>
-    <hyperlink ref="G16" r:id="rId59" display="https://data.gov.tw/datasets/search?qs=dtid:493 "/>
-    <hyperlink ref="G17" r:id="rId60" display="https://data.gov.tw/datasets/search?qs=dtid:509 "/>
-    <hyperlink ref="G18" r:id="rId61" display="https://data.gov.tw/datasets/search?qs=dtid:498 "/>
-    <hyperlink ref="G19" r:id="rId62" display="https://data.gov.tw/datasets/search?qs=dtid:517 "/>
-    <hyperlink ref="G20" r:id="rId63" display="https://data.gov.tw/datasets/search?qs=dtid:489 "/>
-    <hyperlink ref="G21" r:id="rId64" display="https://data.gov.tw/datasets/search?qs=dtid:491 "/>
-    <hyperlink ref="G22" r:id="rId65" display="https://data.gov.tw/datasets/search?qs=dtid:499 "/>
-    <hyperlink ref="G23" r:id="rId66" display="https://data.gov.tw/datasets/search?qs=dtid:507 "/>
-    <hyperlink ref="G24" r:id="rId67" display="https://data.gov.tw/datasets/search?qs=dtid:504 "/>
-    <hyperlink ref="G25" r:id="rId68" display="https://data.gov.tw/datasets/search?qs=dtid:484 "/>
-    <hyperlink ref="G26" r:id="rId69" display="https://data.gov.tw/datasets/search?qs=dtid:486 "/>
-    <hyperlink ref="G27" r:id="rId70" display="https://data.gov.tw/datasets/search?qs=dtid:503 "/>
-    <hyperlink ref="G28" r:id="rId71" display="https://data.gov.tw/datasets/search?qs=dtid:506 "/>
-    <hyperlink ref="G29" r:id="rId72" display="https://data.gov.tw/datasets/search?qs=dtid:502 "/>
-    <hyperlink ref="G30" r:id="rId73" display="https://data.gov.tw/datasets/search?qs=dtid:518 "/>
-    <hyperlink ref="G31" r:id="rId74" display="https://data.gov.tw/datasets/search?qs=dtid:519 "/>
-    <hyperlink ref="G32" r:id="rId75" display="https://data.gov.tw/datasets/search?qs=dtid:495 "/>
-    <hyperlink ref="G33" r:id="rId76" display="https://data.gov.tw/datasets/search?qs=dtid:487 "/>
-    <hyperlink ref="G34" r:id="rId77" display="https://data.gov.tw/datasets/search?qs=dtid:488 "/>
-    <hyperlink ref="G35" r:id="rId78" display="https://data.gov.tw/datasets/search?qs=dtid:496 "/>
-    <hyperlink ref="G36" r:id="rId79" display="https://data.gov.tw/datasets/search?qs=dtid:500 "/>
-    <hyperlink ref="G37" r:id="rId80" display="https://data.gov.tw/datasets/search?qs=dtid:508 "/>
-    <hyperlink ref="G38" r:id="rId81" display="https://data.gov.tw/datasets/search?qs=dtid:737 "/>
-    <hyperlink ref="G39" r:id="rId82" display="https://data.gov.tw/datasets/search?qs=dtid:16720 "/>
-    <hyperlink ref="G40" r:id="rId83" display="https://data.gov.tw/datasets/search?qs=dtid:847 "/>
-    <hyperlink ref="G41" r:id="rId84" display="https://data.gov.tw/datasets/search?qs=dtid:807 "/>
-    <hyperlink ref="G42" r:id="rId85" display="https://data.gov.tw/datasets/search?qs=dtid:505 "/>
-    <hyperlink ref="G43" r:id="rId86" display="https://data.gov.tw/datasets/search?qs=dtid:797 "/>
-    <hyperlink ref="G44" r:id="rId87" display="https://data.gov.tw/datasets/search?qs=dtid:748 "/>
-    <hyperlink ref="G45" r:id="rId88" display="https://data.gov.tw/datasets/search?qs=dtid:832 "/>
-    <hyperlink ref="G46" r:id="rId89" display="https://data.gov.tw/datasets/search?qs=dtid:798 "/>
-    <hyperlink ref="G47" r:id="rId90" display="https://data.gov.tw/datasets/search?qs=dtid:806 "/>
-    <hyperlink ref="G48" r:id="rId91" display="https://data.gov.tw/datasets/search?qs=dtid:772 "/>
-    <hyperlink ref="G49" r:id="rId92" display="https://data.gov.tw/datasets/search?qs=dtid:837 "/>
-    <hyperlink ref="G50" r:id="rId93" display="https://data.gov.tw/datasets/search?qs=dtid:821 "/>
-    <hyperlink ref="G51" r:id="rId94" display="https://data.gov.tw/datasets/search?qs=dtid:827 "/>
-    <hyperlink ref="G52" r:id="rId95" display="https://data.gov.tw/datasets/search?qs=dtid:818 "/>
-    <hyperlink ref="G53" r:id="rId96" display="https://data.gov.tw/datasets/search?qs=dtid:770 "/>
-    <hyperlink ref="G54" r:id="rId97" display="https://data.gov.tw/datasets/search?qs=dtid:802 "/>
-    <hyperlink ref="G55" r:id="rId98" display="https://data.gov.tw/datasets/search?qs=dtid:786 "/>
-    <hyperlink ref="G56" r:id="rId99" display="https://data.gov.tw/datasets/search?qs=dtid:773 "/>
-    <hyperlink ref="G57" r:id="rId100" display="https://data.gov.tw/datasets/search?qs=dtid:736 "/>
-    <hyperlink ref="G58" r:id="rId101" display="https://data.gov.tw/datasets/search?qs=dtid:691 "/>
-    <hyperlink ref="G59" r:id="rId102" display="https://data.gov.tw/datasets/search?qs=dtid:729 "/>
-    <hyperlink ref="G60" r:id="rId103" display="https://data.gov.tw/datasets/search?qs=dtid:826 "/>
-    <hyperlink ref="G61" r:id="rId104" display="https://data.gov.tw/datasets/search?qs=dtid:820 "/>
-    <hyperlink ref="G62" r:id="rId105" display="https://data.gov.tw/datasets/search?qs=dtid:842 "/>
-    <hyperlink ref="G63" r:id="rId106" display="https://data.gov.tw/datasets/search?qs=dtid:728 "/>
-    <hyperlink ref="G64" r:id="rId107"/>
-    <hyperlink ref="D64" r:id="rId108"/>
+    <hyperlink ref="G6" r:id="rId48" display="https://data.gov.tw/datasets/search?qs=dtid:739 "/>
+    <hyperlink ref="G7" r:id="rId49" display="https://data.gov.tw/datasets/search?qs=dtid:428 "/>
+    <hyperlink ref="G8" r:id="rId50" display="https://data.gov.tw/datasets/search?qs=dtid:429 "/>
+    <hyperlink ref="G9" r:id="rId51" display="https://data.gov.tw/datasets/search?qs=dtid:430 "/>
+    <hyperlink ref="G11" r:id="rId52" display="https://data.gov.tw/datasets/search?qs=dtid:431 "/>
+    <hyperlink ref="G12" r:id="rId53" display="https://data.gov.tw/datasets/search?qs=dtid:432 "/>
+    <hyperlink ref="G13" r:id="rId54" display="https://data.gov.tw/datasets/search?qs=dtid:440 "/>
+    <hyperlink ref="G14" r:id="rId55" display="https://data.gov.tw/datasets/search?qs=dtid:442 "/>
+    <hyperlink ref="G15" r:id="rId56" display="https://data.gov.tw/datasets/search?qs=dtid:443 "/>
+    <hyperlink ref="G16" r:id="rId57" display="https://data.gov.tw/datasets/search?qs=dtid:466 "/>
+    <hyperlink ref="G17" r:id="rId58" display="https://data.gov.tw/datasets/search?qs=dtid:497 "/>
+    <hyperlink ref="G18" r:id="rId59" display="https://data.gov.tw/datasets/search?qs=dtid:493 "/>
+    <hyperlink ref="G19" r:id="rId60" display="https://data.gov.tw/datasets/search?qs=dtid:509 "/>
+    <hyperlink ref="G20" r:id="rId61" display="https://data.gov.tw/datasets/search?qs=dtid:498 "/>
+    <hyperlink ref="G21" r:id="rId62" display="https://data.gov.tw/datasets/search?qs=dtid:517 "/>
+    <hyperlink ref="G22" r:id="rId63" display="https://data.gov.tw/datasets/search?qs=dtid:489 "/>
+    <hyperlink ref="G23" r:id="rId64" display="https://data.gov.tw/datasets/search?qs=dtid:491 "/>
+    <hyperlink ref="G24" r:id="rId65" display="https://data.gov.tw/datasets/search?qs=dtid:499 "/>
+    <hyperlink ref="G25" r:id="rId66" display="https://data.gov.tw/datasets/search?qs=dtid:507 "/>
+    <hyperlink ref="G26" r:id="rId67" display="https://data.gov.tw/datasets/search?qs=dtid:504 "/>
+    <hyperlink ref="G27" r:id="rId68" display="https://data.gov.tw/datasets/search?qs=dtid:484 "/>
+    <hyperlink ref="G28" r:id="rId69" display="https://data.gov.tw/datasets/search?qs=dtid:486 "/>
+    <hyperlink ref="G29" r:id="rId70" display="https://data.gov.tw/datasets/search?qs=dtid:503 "/>
+    <hyperlink ref="G30" r:id="rId71" display="https://data.gov.tw/datasets/search?qs=dtid:506 "/>
+    <hyperlink ref="G31" r:id="rId72" display="https://data.gov.tw/datasets/search?qs=dtid:502 "/>
+    <hyperlink ref="G32" r:id="rId73" display="https://data.gov.tw/datasets/search?qs=dtid:518 "/>
+    <hyperlink ref="G33" r:id="rId74" display="https://data.gov.tw/datasets/search?qs=dtid:519 "/>
+    <hyperlink ref="G34" r:id="rId75" display="https://data.gov.tw/datasets/search?qs=dtid:495 "/>
+    <hyperlink ref="G35" r:id="rId76" display="https://data.gov.tw/datasets/search?qs=dtid:487 "/>
+    <hyperlink ref="G36" r:id="rId77" display="https://data.gov.tw/datasets/search?qs=dtid:488 "/>
+    <hyperlink ref="G37" r:id="rId78" display="https://data.gov.tw/datasets/search?qs=dtid:496 "/>
+    <hyperlink ref="G38" r:id="rId79" display="https://data.gov.tw/datasets/search?qs=dtid:500 "/>
+    <hyperlink ref="G39" r:id="rId80" display="https://data.gov.tw/datasets/search?qs=dtid:508 "/>
+    <hyperlink ref="G40" r:id="rId81" display="https://data.gov.tw/datasets/search?qs=dtid:737 "/>
+    <hyperlink ref="G41" r:id="rId82" display="https://data.gov.tw/datasets/search?qs=dtid:16720 "/>
+    <hyperlink ref="G42" r:id="rId83" display="https://data.gov.tw/datasets/search?qs=dtid:847 "/>
+    <hyperlink ref="G43" r:id="rId84" display="https://data.gov.tw/datasets/search?qs=dtid:807 "/>
+    <hyperlink ref="G44" r:id="rId85" display="https://data.gov.tw/datasets/search?qs=dtid:505 "/>
+    <hyperlink ref="G45" r:id="rId86" display="https://data.gov.tw/datasets/search?qs=dtid:797 "/>
+    <hyperlink ref="G46" r:id="rId87" display="https://data.gov.tw/datasets/search?qs=dtid:748 "/>
+    <hyperlink ref="G47" r:id="rId88" display="https://data.gov.tw/datasets/search?qs=dtid:832 "/>
+    <hyperlink ref="G48" r:id="rId89" display="https://data.gov.tw/datasets/search?qs=dtid:798 "/>
+    <hyperlink ref="G49" r:id="rId90" display="https://data.gov.tw/datasets/search?qs=dtid:806 "/>
+    <hyperlink ref="G50" r:id="rId91" display="https://data.gov.tw/datasets/search?qs=dtid:772 "/>
+    <hyperlink ref="G51" r:id="rId92" display="https://data.gov.tw/datasets/search?qs=dtid:837 "/>
+    <hyperlink ref="G52" r:id="rId93" display="https://data.gov.tw/datasets/search?qs=dtid:821 "/>
+    <hyperlink ref="G53" r:id="rId94" display="https://data.gov.tw/datasets/search?qs=dtid:827 "/>
+    <hyperlink ref="G54" r:id="rId95" display="https://data.gov.tw/datasets/search?qs=dtid:818 "/>
+    <hyperlink ref="G55" r:id="rId96" display="https://data.gov.tw/datasets/search?qs=dtid:770 "/>
+    <hyperlink ref="G56" r:id="rId97" display="https://data.gov.tw/datasets/search?qs=dtid:802 "/>
+    <hyperlink ref="G57" r:id="rId98" display="https://data.gov.tw/datasets/search?qs=dtid:786 "/>
+    <hyperlink ref="G58" r:id="rId99" display="https://data.gov.tw/datasets/search?qs=dtid:773 "/>
+    <hyperlink ref="G59" r:id="rId100" display="https://data.gov.tw/datasets/search?qs=dtid:736 "/>
+    <hyperlink ref="G60" r:id="rId101" display="https://data.gov.tw/datasets/search?qs=dtid:691 "/>
+    <hyperlink ref="G61" r:id="rId102" display="https://data.gov.tw/datasets/search?qs=dtid:729 "/>
+    <hyperlink ref="G62" r:id="rId103" display="https://data.gov.tw/datasets/search?qs=dtid:826 "/>
+    <hyperlink ref="G63" r:id="rId104" display="https://data.gov.tw/datasets/search?qs=dtid:820 "/>
+    <hyperlink ref="G64" r:id="rId105" display="https://data.gov.tw/datasets/search?qs=dtid:842 "/>
+    <hyperlink ref="G65" r:id="rId106" display="https://data.gov.tw/datasets/search?qs=dtid:728 "/>
+    <hyperlink ref="G66" r:id="rId107"/>
+    <hyperlink ref="D66" r:id="rId108"/>
+    <hyperlink ref="F5" r:id="rId109"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" copies="0" r:id="rId109"/>
+  <pageSetup paperSize="9" orientation="portrait" copies="0" r:id="rId110"/>
   <ignoredErrors>
-    <ignoredError sqref="H3:H64" numberStoredAsText="1"/>
+    <ignoredError sqref="H11:H66 H6:H9 H3:H4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -4512,7 +4643,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12:XFD12"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.77734375" defaultRowHeight="15.6"/>
@@ -5075,8 +5206,8 @@
   <dimension ref="A1:F349"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A122" sqref="A122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>

</xml_diff>